<commit_message>
include analytical uncertainty in isotope plots and tables
</commit_message>
<xml_diff>
--- a/data/2017_Silverman_et_al-isotope_data.xlsx
+++ b/data/2017_Silverman_et_al-isotope_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">organism</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t xml:space="preserve">eps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eps_sigma_analytical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eps_sigma_absolute</t>
   </si>
   <si>
     <t xml:space="preserve">A. cylindrica</t>
@@ -374,10 +380,16 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
         <v>0.1</v>
@@ -388,10 +400,16 @@
       <c r="D2" t="n">
         <v>-1.81347249285241</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>0.1</v>
@@ -402,10 +420,16 @@
       <c r="D3" t="n">
         <v>-1.79801111006759</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
         <v>0.1</v>
@@ -416,10 +440,16 @@
       <c r="D4" t="n">
         <v>-1.92185460877486</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
         <v>0.1</v>
@@ -430,10 +460,16 @@
       <c r="D5" t="n">
         <v>-1.90087788711683</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
         <v>0.3</v>
@@ -444,10 +480,16 @@
       <c r="D6" t="n">
         <v>-1.80292538053808</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
         <v>0.3</v>
@@ -458,10 +500,16 @@
       <c r="D7" t="n">
         <v>-2.15837425231841</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>0.3</v>
@@ -472,10 +520,16 @@
       <c r="D8" t="n">
         <v>-2.16795848525289</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" t="n">
         <v>0.3</v>
@@ -486,10 +540,16 @@
       <c r="D9" t="n">
         <v>-2.08727132493474</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" t="n">
         <v>0.5</v>
@@ -500,10 +560,16 @@
       <c r="D10" t="n">
         <v>-2.32792867435773</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" t="n">
         <v>0.5</v>
@@ -514,10 +580,16 @@
       <c r="D11" t="n">
         <v>-2.28973903449105</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" t="n">
         <v>0.5</v>
@@ -528,10 +600,16 @@
       <c r="D12" t="n">
         <v>-2.19531482444521</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" t="n">
         <v>0.5</v>
@@ -542,10 +620,16 @@
       <c r="D13" t="n">
         <v>-2.2153863618197</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" t="n">
         <v>0.8</v>
@@ -556,10 +640,16 @@
       <c r="D14" t="n">
         <v>-2.43352601990378</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" t="n">
         <v>0.8</v>
@@ -570,10 +660,16 @@
       <c r="D15" t="n">
         <v>-2.43620742349223</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" t="n">
         <v>0.8</v>
@@ -584,10 +680,16 @@
       <c r="D16" t="n">
         <v>-2.43172988278695</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
         <v>0.8</v>
@@ -598,10 +700,16 @@
       <c r="D17" t="n">
         <v>-2.4974344596832</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18" t="n">
         <v>0.1</v>
@@ -612,10 +720,16 @@
       <c r="D18" t="n">
         <v>-2.19807152035206</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B19" t="n">
         <v>0.1</v>
@@ -626,10 +740,16 @@
       <c r="D19" t="n">
         <v>-2.20084957482328</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B20" t="n">
         <v>0.3</v>
@@ -640,10 +760,16 @@
       <c r="D20" t="n">
         <v>-2.25350175797484</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B21" t="n">
         <v>0.3</v>
@@ -654,10 +780,16 @@
       <c r="D21" t="n">
         <v>-2.32185405061599</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B22" t="n">
         <v>0.3</v>
@@ -668,10 +800,16 @@
       <c r="D22" t="n">
         <v>-2.3296287634504</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B23" t="n">
         <v>0.5</v>
@@ -682,10 +820,16 @@
       <c r="D23" t="n">
         <v>-2.28381740809395</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B24" t="n">
         <v>0.5</v>
@@ -696,10 +840,16 @@
       <c r="D24" t="n">
         <v>-2.44261572530643</v>
       </c>
+      <c r="E24" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B25" t="n">
         <v>0.5</v>
@@ -710,10 +860,16 @@
       <c r="D25" t="n">
         <v>-2.41263011082399</v>
       </c>
+      <c r="E25" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B26" t="n">
         <v>0.8</v>
@@ -724,10 +880,16 @@
       <c r="D26" t="n">
         <v>-2.53990096400585</v>
       </c>
+      <c r="E26" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B27" t="n">
         <v>0.8</v>
@@ -738,10 +900,16 @@
       <c r="D27" t="n">
         <v>-2.42956135278147</v>
       </c>
+      <c r="E27" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B28" t="n">
         <v>0.8</v>
@@ -751,6 +919,12 @@
       </c>
       <c r="D28" t="n">
         <v>-2.42657413144225</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.084195259341794</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>